<commit_message>
getting code of tipo_impuesto and tipo_acto_tramite
</commit_message>
<xml_diff>
--- a/storage/app/public/users/jose.jdgo97/PERSUASIVO.xlsx
+++ b/storage/app/public/users/jose.jdgo97/PERSUASIVO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\www\LARAVEL\versiones cam\multimedia_cam4\public\storage\users\jose.jdgo97\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\www\LARAVEL\versiones cam\multimedia_cam3\public\storage\users\jose.jdgo97\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1E8BB5-62BC-4BD5-818E-F1A280574D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA868D2B-2940-4852-9F1F-C4BFEC04A2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -687,7 +687,7 @@
   <dimension ref="A1:R415"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,7 +853,7 @@
         <v>15</v>
       </c>
       <c r="O5" s="18">
-        <v>45726</v>
+        <v>45719</v>
       </c>
       <c r="P5" s="19">
         <v>0.14583333333333334</v>

</xml_diff>